<commit_message>
Added new ss capture method and changed Driver to static
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/UITestData/QA_TEST_DATA.xlsx
+++ b/src/test/resources/testData/UITestData/QA_TEST_DATA.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Komal.Phadtare\MyWorkSpace\HybridFramework\src\test\resources\testData\UITestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9DEBE8-1FA4-41B0-9D8F-8107C3642569}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15BEB2E9-CD8D-487B-AFDA-A8B6CAA4C34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC01" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t>userName</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t xml:space="preserve">And User should not get logged in </t>
+  </si>
+  <si>
+    <t>Feature: Place Order</t>
+  </si>
+  <si>
+    <t>Scenario: Place order on SauceDemo</t>
   </si>
 </sst>
 </file>
@@ -717,7 +723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E648B68-8507-4F9D-98A7-13659DF19D79}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -930,10 +936,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612D4189-A6F4-4582-856E-6B1D21CBA882}">
-  <dimension ref="A2:B10"/>
+  <dimension ref="A2:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -984,6 +990,16 @@
         <v>52</v>
       </c>
     </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>